<commit_message>
this is my 3rd commit
</commit_message>
<xml_diff>
--- a/src/test/java/com/sysmatech/TestData/DemoFor.xlsx
+++ b/src/test/java/com/sysmatech/TestData/DemoFor.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>SelectCompany</t>
   </si>
@@ -66,29 +71,32 @@
     <t>…..</t>
   </si>
   <si>
-    <t>Rakesh1111</t>
-  </si>
-  <si>
-    <t>Asset11111</t>
-  </si>
-  <si>
-    <t>rakeshSupplier</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>RakeshModel123</t>
+    <t>Rakesh11</t>
+  </si>
+  <si>
+    <t>AutomationModel</t>
+  </si>
+  <si>
+    <t>AutomationAsset</t>
+  </si>
+  <si>
+    <t>AutomationSupplier</t>
+  </si>
+  <si>
+    <t>Parola</t>
+  </si>
+  <si>
+    <t>us-9877</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +156,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -194,7 +210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,9 +242,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,6 +277,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,14 +453,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -453,7 +471,7 @@
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -505,19 +523,19 @@
         <v>7865</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5">
         <v>44945</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="4">
         <v>1234</v>
@@ -532,7 +550,48 @@
         <v>15</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4">
+        <v>7865</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5">
+        <v>44946</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1234</v>
+      </c>
+      <c r="J3" s="4">
+        <v>35000</v>
+      </c>
+      <c r="K3" s="4">
+        <v>6</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -541,24 +600,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>